<commit_message>
Addressed Typos in .xlsx file
</commit_message>
<xml_diff>
--- a/Backend/database/restaurants_menus.xlsx
+++ b/Backend/database/restaurants_menus.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erin/Desktop/Senior Proj/Backend/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E584F8F6-1D7B-0D4F-B65A-E7ACAD78A60E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E33A45E-4551-E84A-856E-7A47300CBCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="18000" activeTab="1" xr2:uid="{3E180D32-923C-C640-8E37-FF46F6D4E035}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="18000" activeTab="10" xr2:uid="{3E180D32-923C-C640-8E37-FF46F6D4E035}"/>
   </bookViews>
   <sheets>
     <sheet name="restaurants" sheetId="1" r:id="rId1"/>
@@ -1914,7 +1914,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="435">
   <si>
     <t>name</t>
   </si>
@@ -2450,12 +2450,6 @@
     <t>Avocado, Imitation Crab, Cucumber, Rice, Nori</t>
   </si>
   <si>
-    <t>Fish, Gluten</t>
-  </si>
-  <si>
-    <t>Gluten, Milk, Soy, Eggs</t>
-  </si>
-  <si>
     <t>Sirloin &amp; Ribs</t>
   </si>
   <si>
@@ -2474,18 +2468,12 @@
     <t>Eggs, Wheat, Soy, Pork, Sesame</t>
   </si>
   <si>
-    <t>Peanuts, Tree Nuts, Gluten, Soy, Eggs, Sesame</t>
-  </si>
-  <si>
     <t>Popcorn Shrimp</t>
   </si>
   <si>
     <t>Shrimp, Milk, Eggs, Wheat, Sesame</t>
   </si>
   <si>
-    <t>Gluten, Soy, Fish, Eggs, Sesame</t>
-  </si>
-  <si>
     <t>Korean Cheese Corn</t>
   </si>
   <si>
@@ -2504,9 +2492,6 @@
     <t>Mushroom, Carrots, Avocado, Cabbage, Lettuce, Tortilla</t>
   </si>
   <si>
-    <t>Wheat, Sesame, Soy</t>
-  </si>
-  <si>
     <t>Roasted Veggie Harvest Soup</t>
   </si>
   <si>
@@ -2531,27 +2516,18 @@
     <t>Tofu, Chili Pesto, Rice, Sesame Seeds, Nori</t>
   </si>
   <si>
-    <t>Fish, Soy, Gluten, Sesame</t>
-  </si>
-  <si>
     <t>Shoyu Paitan</t>
   </si>
   <si>
     <t>Chicken Broth, Shoyu Tare, Tonkotsu Noodles, Chicken, Scallions, Garlic Oil, Nori</t>
   </si>
   <si>
-    <t>Egg, Fish, Soy, Gluten</t>
-  </si>
-  <si>
     <t>Spicy Miso</t>
   </si>
   <si>
     <t>Chicken Broth, Red Miso, Chili Oil, Tonkusen Noodles, Chashu, Mushrooms, Scallions</t>
   </si>
   <si>
-    <t>Egg, Sesame, Soy, Gluten</t>
-  </si>
-  <si>
     <t>Cheese Pizza</t>
   </si>
   <si>
@@ -2657,15 +2633,9 @@
     <t>Bread, Bacon, Eggs, Hash Brown, Cheese</t>
   </si>
   <si>
-    <t>Gluten, Egg, Milk</t>
-  </si>
-  <si>
     <t>Cheese Quesadillas</t>
   </si>
   <si>
-    <t>Gluten, Milk, Tomato</t>
-  </si>
-  <si>
     <t>Cheese, Corn</t>
   </si>
   <si>
@@ -2681,9 +2651,6 @@
     <t>Kale Salad</t>
   </si>
   <si>
-    <t>Gluten, Soy</t>
-  </si>
-  <si>
     <t>Kale, Miso, Tempura, Kale, Raisins, Avocado</t>
   </si>
   <si>
@@ -2699,24 +2666,15 @@
     <t>Shrimp, Coconut, Rice, Microgreens, Lemon, Yuzu Kosho Butter</t>
   </si>
   <si>
-    <t>Shellfish, Tree Nuts, Gluten, Sesame, Soy, Fish</t>
-  </si>
-  <si>
     <t>Kimchi Fried Rice</t>
   </si>
   <si>
     <t>Chicken, Scallion, Bacon, Egg, Cabbage, Onion, Shallots, Kimchi, Chili</t>
   </si>
   <si>
-    <t>Egg, Fish, Gluten, Soy, Sesame</t>
-  </si>
-  <si>
     <t>Salmon, Balsamic Vinegar, Pesto, Tomatoes, Microgreens</t>
   </si>
   <si>
-    <t>Fish, Tree nuts</t>
-  </si>
-  <si>
     <t>Ravioletti Tricolore</t>
   </si>
   <si>
@@ -2960,9 +2918,6 @@
     <t>Oat</t>
   </si>
   <si>
-    <t>Gluten</t>
-  </si>
-  <si>
     <t>Almond</t>
   </si>
   <si>
@@ -2972,51 +2927,9 @@
     <t>Skim</t>
   </si>
   <si>
-    <t>Soy</t>
-  </si>
-  <si>
     <t>Wheat, Eggs, Milk</t>
   </si>
   <si>
-    <t>Gluten, Milk, Tomato, Fish</t>
-  </si>
-  <si>
-    <t>Gluten, Soy, Milk, Eggs, Sesame, Fish</t>
-  </si>
-  <si>
-    <t>Milk, Sesame, Soy, Gluten</t>
-  </si>
-  <si>
-    <t>Gluten, Eggs, Milk</t>
-  </si>
-  <si>
-    <t>Milk, Egg, Gluten</t>
-  </si>
-  <si>
-    <t>Peanuts, Gluten, Milk, Eggs</t>
-  </si>
-  <si>
-    <t>Milk, Gluten</t>
-  </si>
-  <si>
-    <t>Gluten, Milk</t>
-  </si>
-  <si>
-    <t>Gluten, Milk, Eggs, Fish</t>
-  </si>
-  <si>
-    <t>Gluten, Milk, Eggs</t>
-  </si>
-  <si>
-    <t>milk, Wheat, Peanuts</t>
-  </si>
-  <si>
-    <t>milk, Wheat, Pecans</t>
-  </si>
-  <si>
-    <t>milk, Wheat</t>
-  </si>
-  <si>
     <t>Salads</t>
   </si>
   <si>
@@ -3041,9 +2954,6 @@
     <t>Chicken, Tomatoes, Garlic, Croutons, Parmesan, Basil, Lemon, Lettuce, Caesar Dressing</t>
   </si>
   <si>
-    <t>Milk, Wheat, Soy, Fish, Egg</t>
-  </si>
-  <si>
     <t>Almond Croissant</t>
   </si>
   <si>
@@ -3182,18 +3092,12 @@
     <t>Add Chopped Bacon</t>
   </si>
   <si>
-    <t>Milk, Egg</t>
-  </si>
-  <si>
     <t>Corn, Onions, Lettuce, Tomatoes, Cilantro, Chicken, Chipotle, Avocado, Flour, Vinegar, Sugar, Salt, Cilantro, Paprika, Pepper, Rice, Water</t>
   </si>
   <si>
     <t>Cranberry Walnut Chicken Salad Sandwich</t>
   </si>
   <si>
-    <t>Egg, Walnut, Wheat</t>
-  </si>
-  <si>
     <t>Chicken, Walnuts, Bread, Tomatoes, Lettuce, Onions, Cranberry, Salt, Pepper, Honey, Celery, Mayonnaise</t>
   </si>
   <si>
@@ -3203,13 +3107,118 @@
     <t>Coconut, Egg, Almond, Vanilla, Cocoa,  Chocolate, Flour, Sugar</t>
   </si>
   <si>
-    <t>Egg, Milk, Almonds, Wheat, Soy</t>
-  </si>
-  <si>
     <t>Frozen Strawberry Lemonade</t>
   </si>
   <si>
     <t>Water, Strawberry, Lemon, Apple, Grape</t>
+  </si>
+  <si>
+    <t>Egg, Milk, Almonds, Wheat, Soybeans</t>
+  </si>
+  <si>
+    <t>Egg, Walnut, Wheat, Celery</t>
+  </si>
+  <si>
+    <t>Milk, Egg, Avocado</t>
+  </si>
+  <si>
+    <t>Strawberry</t>
+  </si>
+  <si>
+    <t>Fruits</t>
+  </si>
+  <si>
+    <t>Milk, Wheat, Garlic</t>
+  </si>
+  <si>
+    <t>Wheat, Milk, Garlic</t>
+  </si>
+  <si>
+    <t>Milk, Wheat, Peanuts</t>
+  </si>
+  <si>
+    <t>Milk, Wheat, Pecans</t>
+  </si>
+  <si>
+    <t>Milk, Wheat, Strawberry</t>
+  </si>
+  <si>
+    <t>Wheat, Milk, Eggs, Shrimp, Garlic</t>
+  </si>
+  <si>
+    <t>Wheat, Milk, Eggs</t>
+  </si>
+  <si>
+    <t>Wheat, Milk, Eggs, Garlic</t>
+  </si>
+  <si>
+    <t>Wheat</t>
+  </si>
+  <si>
+    <t>Wheat, Sesame, Soybeans</t>
+  </si>
+  <si>
+    <t>Soybeans</t>
+  </si>
+  <si>
+    <t>Fish, Pine Nuts</t>
+  </si>
+  <si>
+    <t>Celery, Garlic</t>
+  </si>
+  <si>
+    <t>Milk, Wheat, Garlic, Soybeans, Fish, Egg</t>
+  </si>
+  <si>
+    <t>Peanuts, Wheat, Milk, Eggs</t>
+  </si>
+  <si>
+    <t>Milk, Egg, Wheat</t>
+  </si>
+  <si>
+    <t>Peanuts, Tree Nuts, Wheat, Soybeans, Eggs, Sesame</t>
+  </si>
+  <si>
+    <t>Wheat, Soybeans, Shrimp, Eggs, Sesame</t>
+  </si>
+  <si>
+    <t>Fish, Soybeans, Wheat, Sesame, Pine Nuts</t>
+  </si>
+  <si>
+    <t>Egg, Sesame, Soybeans, Wheat</t>
+  </si>
+  <si>
+    <t>Milk, Sesame, Soybeans, Wheat</t>
+  </si>
+  <si>
+    <t>Wheat, Soybeans</t>
+  </si>
+  <si>
+    <t>Egg, Fish, Wheat, Soybeans, Sesame</t>
+  </si>
+  <si>
+    <t>Shellfish, Tree Nuts, Wheat, Sesame, Soybeans, Fish, Coconut</t>
+  </si>
+  <si>
+    <t>Wheat, Soybeans, Milk, Eggs, Sesame, Fish, Garlic</t>
+  </si>
+  <si>
+    <t>Egg, Fish, Soybeans, Wheat, Garlic</t>
+  </si>
+  <si>
+    <t>Wheat, Milk, Tomato</t>
+  </si>
+  <si>
+    <t>Wheat, Milk, Tomato, Fish</t>
+  </si>
+  <si>
+    <t>Fish, Wheat, Crab</t>
+  </si>
+  <si>
+    <t>Wheat, Egg, Milk</t>
+  </si>
+  <si>
+    <t>Wheat, Milk, Soybeans, Eggs</t>
   </si>
 </sst>
 </file>
@@ -3425,7 +3434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
@@ -3455,7 +3464,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -3463,233 +3471,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="101">
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="6"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color theme="6"/>
-        </left>
-        <right style="thin">
-          <color theme="6"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri Light"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-      </font>
-    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4601,6 +4382,188 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
         <top style="thin">
           <color theme="6"/>
@@ -4608,10 +4571,55 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+      </font>
+    </dxf>
+    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color auto="1"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="6"/>
+        <name val="Calibri Light"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="6"/>
+        </left>
+        <right style="thin">
+          <color theme="6"/>
+        </right>
+        <top/>
+        <bottom/>
       </border>
     </dxf>
     <dxf>
@@ -5281,7 +5289,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{9891CE72-5244-1547-9248-A1EF2B8A5D67}" name="Table15" displayName="Table15" ref="A1:O23" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0" headerRowBorderDxfId="70" tableBorderDxfId="69">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{9891CE72-5244-1547-9248-A1EF2B8A5D67}" name="Table15" displayName="Table15" ref="A1:O23" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67">
   <autoFilter ref="A1:O23" xr:uid="{9891CE72-5244-1547-9248-A1EF2B8A5D67}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5300,28 +5308,28 @@
     <filterColumn colId="14" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{7A1890C9-AB4A-7146-811A-C813973AB96C}" name="category" dataDxfId="16"/>
-    <tableColumn id="2" xr3:uid="{2811EC5D-2FA2-B94B-9037-0F2890E3C353}" name="sub_category" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{13F6EF02-4055-4649-A54C-A3179AF1ACBD}" name="name" dataDxfId="14"/>
-    <tableColumn id="4" xr3:uid="{1E116047-F4A1-E948-8699-340BB8A5990F}" name="price" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{E4D9ABBB-F4ED-8447-A06A-52915DE57D81}" name="ingredients" dataDxfId="12"/>
-    <tableColumn id="6" xr3:uid="{729360A1-021A-E249-9F7C-6423FB565FCB}" name="allergens" dataDxfId="11"/>
-    <tableColumn id="7" xr3:uid="{6952B167-C1B3-E44C-8AE7-FCCE8B00E1A0}" name="description" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{0F88A1B4-0A7C-5247-A501-A46FF999F32A}" name="image_filename" dataDxfId="9"/>
-    <tableColumn id="8" xr3:uid="{0A8C9853-C81D-1347-9881-1F2382338D70}" name="option_group_id" dataDxfId="8"/>
-    <tableColumn id="9" xr3:uid="{CF37D21B-E29E-D14F-A46E-EAF0290C2E87}" name="option_group_description" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{20D6CFAA-C2FB-244E-B557-47E401B341B7}" name="option_min_quantity" dataDxfId="6"/>
-    <tableColumn id="11" xr3:uid="{EC75C3D1-0B39-5240-AB35-E38AF020853B}" name="option_max_quantity" dataDxfId="5"/>
-    <tableColumn id="12" xr3:uid="{67CE16D7-5D55-8646-9A87-813440C3C10D}" name="option_item_name" dataDxfId="4"/>
-    <tableColumn id="13" xr3:uid="{178226DE-7217-2C4B-8C43-7AC79CE6C9DC}" name="extra_price" dataDxfId="3"/>
-    <tableColumn id="14" xr3:uid="{C76EBB38-1E3D-0B41-8DB5-30CD32A713E9}" name="option_allergens" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{7A1890C9-AB4A-7146-811A-C813973AB96C}" name="category" dataDxfId="66"/>
+    <tableColumn id="2" xr3:uid="{2811EC5D-2FA2-B94B-9037-0F2890E3C353}" name="sub_category" dataDxfId="65"/>
+    <tableColumn id="3" xr3:uid="{13F6EF02-4055-4649-A54C-A3179AF1ACBD}" name="name" dataDxfId="64"/>
+    <tableColumn id="4" xr3:uid="{1E116047-F4A1-E948-8699-340BB8A5990F}" name="price" dataDxfId="63"/>
+    <tableColumn id="5" xr3:uid="{E4D9ABBB-F4ED-8447-A06A-52915DE57D81}" name="ingredients" dataDxfId="62"/>
+    <tableColumn id="6" xr3:uid="{729360A1-021A-E249-9F7C-6423FB565FCB}" name="allergens" dataDxfId="61"/>
+    <tableColumn id="7" xr3:uid="{6952B167-C1B3-E44C-8AE7-FCCE8B00E1A0}" name="description" dataDxfId="60"/>
+    <tableColumn id="15" xr3:uid="{0F88A1B4-0A7C-5247-A501-A46FF999F32A}" name="image_filename" dataDxfId="59"/>
+    <tableColumn id="8" xr3:uid="{0A8C9853-C81D-1347-9881-1F2382338D70}" name="option_group_id" dataDxfId="58"/>
+    <tableColumn id="9" xr3:uid="{CF37D21B-E29E-D14F-A46E-EAF0290C2E87}" name="option_group_description" dataDxfId="57"/>
+    <tableColumn id="10" xr3:uid="{20D6CFAA-C2FB-244E-B557-47E401B341B7}" name="option_min_quantity" dataDxfId="56"/>
+    <tableColumn id="11" xr3:uid="{EC75C3D1-0B39-5240-AB35-E38AF020853B}" name="option_max_quantity" dataDxfId="55"/>
+    <tableColumn id="12" xr3:uid="{67CE16D7-5D55-8646-9A87-813440C3C10D}" name="option_item_name" dataDxfId="54"/>
+    <tableColumn id="13" xr3:uid="{178226DE-7217-2C4B-8C43-7AC79CE6C9DC}" name="extra_price" dataDxfId="53"/>
+    <tableColumn id="14" xr3:uid="{C76EBB38-1E3D-0B41-8DB5-30CD32A713E9}" name="option_allergens" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AFB4B9C8-896F-2B4C-9AEC-68AD2E00C8C0}" name="Table14" displayName="Table14" ref="A1:O5" totalsRowShown="0" headerRowDxfId="68" headerRowBorderDxfId="67" tableBorderDxfId="66">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AFB4B9C8-896F-2B4C-9AEC-68AD2E00C8C0}" name="Table14" displayName="Table14" ref="A1:O5" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A1:O5" xr:uid="{AFB4B9C8-896F-2B4C-9AEC-68AD2E00C8C0}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5361,7 +5369,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7F42674C-F8E2-BD46-B0CD-6C935E6CF276}" name="Table13" displayName="Table13" ref="A1:O4" totalsRowShown="0" headerRowDxfId="65" headerRowBorderDxfId="64" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7F42674C-F8E2-BD46-B0CD-6C935E6CF276}" name="Table13" displayName="Table13" ref="A1:O4" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46">
   <autoFilter ref="A1:O4" xr:uid="{7F42674C-F8E2-BD46-B0CD-6C935E6CF276}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5401,7 +5409,7 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{53A31204-2F15-774A-9217-6321151D9A7C}" name="Table12" displayName="Table12" ref="A1:O9" totalsRowShown="0" headerRowDxfId="62" headerRowBorderDxfId="61" tableBorderDxfId="60">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{53A31204-2F15-774A-9217-6321151D9A7C}" name="Table12" displayName="Table12" ref="A1:O9" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A1:O9" xr:uid="{53A31204-2F15-774A-9217-6321151D9A7C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5441,7 +5449,7 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{889E6C16-6078-5B43-9A22-05E9C269B41C}" name="Table11" displayName="Table11" ref="A1:O5" totalsRowShown="0" headerRowDxfId="59" headerRowBorderDxfId="58" tableBorderDxfId="57">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{889E6C16-6078-5B43-9A22-05E9C269B41C}" name="Table11" displayName="Table11" ref="A1:O5" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A1:O5" xr:uid="{889E6C16-6078-5B43-9A22-05E9C269B41C}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5462,10 +5470,10 @@
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{46E9298D-E0DE-4F41-B170-BB41C73F0E68}" name="category"/>
     <tableColumn id="2" xr3:uid="{407D958C-F9E3-D54E-BF4E-13513B591B57}" name="sub_category"/>
-    <tableColumn id="3" xr3:uid="{DE42F71D-9F4A-0C43-8E7F-A3E7CFD1FF8B}" name="name" dataDxfId="56"/>
-    <tableColumn id="4" xr3:uid="{731A01EE-AE08-4046-ACE5-EA8AD56D05FC}" name="price" dataDxfId="55"/>
-    <tableColumn id="5" xr3:uid="{6AA97102-D666-5D42-9301-6D9B2A44C096}" name="ingredients" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{17799845-783E-FF4E-AA41-6EEB72ACDFED}" name="allergens" dataDxfId="53"/>
+    <tableColumn id="3" xr3:uid="{DE42F71D-9F4A-0C43-8E7F-A3E7CFD1FF8B}" name="name" dataDxfId="39"/>
+    <tableColumn id="4" xr3:uid="{731A01EE-AE08-4046-ACE5-EA8AD56D05FC}" name="price" dataDxfId="38"/>
+    <tableColumn id="5" xr3:uid="{6AA97102-D666-5D42-9301-6D9B2A44C096}" name="ingredients" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{17799845-783E-FF4E-AA41-6EEB72ACDFED}" name="allergens" dataDxfId="36"/>
     <tableColumn id="7" xr3:uid="{67F2BD87-63C4-BA48-99BB-7096689B4031}" name="description"/>
     <tableColumn id="15" xr3:uid="{EA26ABCC-1C57-574A-B0ED-5D634C842F2D}" name="image_filename"/>
     <tableColumn id="8" xr3:uid="{78F26E54-AC1C-174F-8DC9-FB2A5BD4C8AE}" name="option_group_id"/>
@@ -5481,7 +5489,7 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{2B8457F3-C4FB-F848-A16E-EF50D38EF95F}" name="Table10" displayName="Table10" ref="A1:O9" totalsRowShown="0" headerRowDxfId="52" dataDxfId="50" headerRowBorderDxfId="51" tableBorderDxfId="49">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{2B8457F3-C4FB-F848-A16E-EF50D38EF95F}" name="Table10" displayName="Table10" ref="A1:O9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32">
   <autoFilter ref="A1:O9" xr:uid="{2B8457F3-C4FB-F848-A16E-EF50D38EF95F}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5500,28 +5508,28 @@
     <filterColumn colId="14" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{2AF5C548-16B2-744F-8EAC-C4192F48F795}" name="category" dataDxfId="48"/>
-    <tableColumn id="2" xr3:uid="{6B520F21-3E72-584F-B983-FD4405910BA6}" name="sub_category" dataDxfId="47"/>
-    <tableColumn id="3" xr3:uid="{E08D164F-A0A9-2340-85EB-A98FADBDE372}" name="name" dataDxfId="46"/>
-    <tableColumn id="4" xr3:uid="{3B8FFE8D-A134-9343-90B3-6223F37EE978}" name="price" dataDxfId="45"/>
-    <tableColumn id="5" xr3:uid="{6DEEC88D-D6DF-E04C-ABEC-D780679D3D52}" name="ingredients" dataDxfId="44"/>
-    <tableColumn id="6" xr3:uid="{8FC18231-C95F-A84B-97B1-0123FBB6AC63}" name="allergens" dataDxfId="43"/>
-    <tableColumn id="7" xr3:uid="{7497A09F-A14B-D84E-B29D-57E516E77278}" name="description" dataDxfId="42"/>
-    <tableColumn id="15" xr3:uid="{74889033-6896-B846-A25C-4698955893F4}" name="image_filename" dataDxfId="41"/>
-    <tableColumn id="8" xr3:uid="{8BE05324-BE97-DA40-9A38-A820201185F3}" name="option_group_id" dataDxfId="40"/>
-    <tableColumn id="9" xr3:uid="{34A16C55-883F-E340-9E39-E621594E59F5}" name="option_group_description" dataDxfId="39"/>
-    <tableColumn id="10" xr3:uid="{F1AA8303-DBB2-7244-9F55-269547E4CA00}" name="option_min_quantity" dataDxfId="38"/>
-    <tableColumn id="11" xr3:uid="{B232C425-0630-1D4D-AA8C-60862AC02781}" name="option_max_quantity" dataDxfId="37"/>
-    <tableColumn id="12" xr3:uid="{EB21D867-EC2A-1046-9372-97B5F5F39552}" name="option_item_name" dataDxfId="36"/>
-    <tableColumn id="13" xr3:uid="{83CFFF5F-DD2A-6849-B86D-92DB38FF7001}" name="extra_price" dataDxfId="35"/>
-    <tableColumn id="14" xr3:uid="{1CFC430A-35A6-3847-A639-DA9CF813A9A8}" name="option_allergens" dataDxfId="34"/>
+    <tableColumn id="1" xr3:uid="{2AF5C548-16B2-744F-8EAC-C4192F48F795}" name="category" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{6B520F21-3E72-584F-B983-FD4405910BA6}" name="sub_category" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{E08D164F-A0A9-2340-85EB-A98FADBDE372}" name="name" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{3B8FFE8D-A134-9343-90B3-6223F37EE978}" name="price" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{6DEEC88D-D6DF-E04C-ABEC-D780679D3D52}" name="ingredients" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{8FC18231-C95F-A84B-97B1-0123FBB6AC63}" name="allergens" dataDxfId="26"/>
+    <tableColumn id="7" xr3:uid="{7497A09F-A14B-D84E-B29D-57E516E77278}" name="description" dataDxfId="25"/>
+    <tableColumn id="15" xr3:uid="{74889033-6896-B846-A25C-4698955893F4}" name="image_filename" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{8BE05324-BE97-DA40-9A38-A820201185F3}" name="option_group_id" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{34A16C55-883F-E340-9E39-E621594E59F5}" name="option_group_description" dataDxfId="22"/>
+    <tableColumn id="10" xr3:uid="{F1AA8303-DBB2-7244-9F55-269547E4CA00}" name="option_min_quantity" dataDxfId="21"/>
+    <tableColumn id="11" xr3:uid="{B232C425-0630-1D4D-AA8C-60862AC02781}" name="option_max_quantity" dataDxfId="20"/>
+    <tableColumn id="12" xr3:uid="{EB21D867-EC2A-1046-9372-97B5F5F39552}" name="option_item_name" dataDxfId="19"/>
+    <tableColumn id="13" xr3:uid="{83CFFF5F-DD2A-6849-B86D-92DB38FF7001}" name="extra_price" dataDxfId="18"/>
+    <tableColumn id="14" xr3:uid="{1CFC430A-35A6-3847-A639-DA9CF813A9A8}" name="option_allergens" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}" name="Table5" displayName="Table5" ref="A1:O50" totalsRowShown="0" headerRowDxfId="33" dataDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}" name="Table5" displayName="Table5" ref="A1:O50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
   <autoFilter ref="A1:O50" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
@@ -5540,21 +5548,21 @@
     <filterColumn colId="14" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{1853C437-6A62-6B47-8C9B-564DEA57939A}" name="category" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{7CC90834-B0D1-C849-9B51-B5D9EA77DAA0}" name="sub_category" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{5FF08993-59DB-6349-A6EA-32533F571FF5}" name="name" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{7CF1E11B-4F70-B44E-872E-BCCD8BFE7D9D}" name="price" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{3BF4A478-AEA5-7A41-B357-48C9836E1C80}" name="ingredients" dataDxfId="27"/>
-    <tableColumn id="6" xr3:uid="{E2E7B27E-AAA8-514A-8148-667D740D3AA7}" name="allergens" dataDxfId="26"/>
-    <tableColumn id="7" xr3:uid="{B1097D52-302C-544C-A429-413DED807F5F}" name="description" dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{1F2AE8F3-03BD-7B45-A4C7-02179D959056}" name="image_filename" dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{49269410-C082-8540-AD51-99931EBA2F5B}" name="option_group_id" dataDxfId="23"/>
-    <tableColumn id="8" xr3:uid="{B8E445A1-F5E1-5047-A344-69C841DD833C}" name="option_group_description" dataDxfId="22"/>
-    <tableColumn id="9" xr3:uid="{21396A92-76A0-2442-B8F3-1DA062E205CC}" name="option_min_quantity" dataDxfId="21"/>
-    <tableColumn id="10" xr3:uid="{557EC8C7-A1C9-F84C-B74C-2B1F02DFEF2A}" name="option_max_quantity" dataDxfId="20"/>
-    <tableColumn id="11" xr3:uid="{E71702D2-99DB-F44C-9D2F-810A07ED5309}" name="option_item_name" dataDxfId="19"/>
-    <tableColumn id="12" xr3:uid="{955FD788-14F2-AA4C-B201-A840E08AD65B}" name="extra_price" dataDxfId="18"/>
-    <tableColumn id="13" xr3:uid="{23C3A0BD-31DD-7249-B139-0E6149C8E21D}" name="option_allergens" dataDxfId="17"/>
+    <tableColumn id="1" xr3:uid="{1853C437-6A62-6B47-8C9B-564DEA57939A}" name="category" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7CC90834-B0D1-C849-9B51-B5D9EA77DAA0}" name="sub_category" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{5FF08993-59DB-6349-A6EA-32533F571FF5}" name="name" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{7CF1E11B-4F70-B44E-872E-BCCD8BFE7D9D}" name="price" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{3BF4A478-AEA5-7A41-B357-48C9836E1C80}" name="ingredients" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{E2E7B27E-AAA8-514A-8148-667D740D3AA7}" name="allergens" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{B1097D52-302C-544C-A429-413DED807F5F}" name="description" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{1F2AE8F3-03BD-7B45-A4C7-02179D959056}" name="image_filename" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{49269410-C082-8540-AD51-99931EBA2F5B}" name="option_group_id" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{B8E445A1-F5E1-5047-A344-69C841DD833C}" name="option_group_description" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{21396A92-76A0-2442-B8F3-1DA062E205CC}" name="option_min_quantity" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{557EC8C7-A1C9-F84C-B74C-2B1F02DFEF2A}" name="option_max_quantity" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{E71702D2-99DB-F44C-9D2F-810A07ED5309}" name="option_item_name" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{955FD788-14F2-AA4C-B201-A840E08AD65B}" name="extra_price" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{23C3A0BD-31DD-7249-B139-0E6149C8E21D}" name="option_allergens" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5942,7 +5950,7 @@
         <v>11</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>12</v>
@@ -10182,25 +10190,25 @@
         <v>124</v>
       </c>
       <c r="K5" s="6" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="L5" s="6" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>385</v>
+        <v>355</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>386</v>
+        <v>356</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>387</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:1024 1031:2048 2055:3072 3079:4096 4103:5120 5127:6144 6151:7168 7175:8192 8199:9216 9223:10240 10247:11264 11271:12288 12295:13312 13319:14336 14343:15360 15367:16384" x14ac:dyDescent="0.25">
@@ -10379,110 +10387,110 @@
     </row>
     <row r="12" spans="1:1024 1031:2048 2055:3072 3079:4096 4103:5120 5127:6144 6151:7168 7175:8192 8199:9216 9223:10240 10247:11264 11271:12288 12295:13312 13319:14336 14343:15360 15367:16384" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>296</v>
+        <v>282</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>297</v>
+        <v>283</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>298</v>
+        <v>284</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>43</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>299</v>
+        <v>285</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>300</v>
+        <v>286</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>301</v>
+        <v>287</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="I12" s="9">
         <v>2033717205</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>394</v>
+        <v>364</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>394</v>
+        <v>364</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>394</v>
+        <v>364</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>394</v>
+        <v>364</v>
       </c>
       <c r="O12" s="6" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="13" spans="1:1024 1031:2048 2055:3072 3079:4096 4103:5120 5127:6144 6151:7168 7175:8192 8199:9216 9223:10240 10247:11264 11271:12288 12295:13312 13319:14336 14343:15360 15367:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>388</v>
+        <v>358</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>389</v>
+        <v>359</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>390</v>
+        <v>360</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="22" t="s">
-        <v>391</v>
+      <c r="E13" s="21" t="s">
+        <v>361</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>392</v>
+        <v>362</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>398</v>
+        <v>368</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="I13" s="21">
+        <v>369</v>
+      </c>
+      <c r="I13">
         <v>3016868388</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>393</v>
+        <v>363</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>393</v>
+        <v>363</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>395</v>
+        <v>365</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>393</v>
+        <v>363</v>
       </c>
       <c r="O13" s="6" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>396</v>
+        <v>366</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>397</v>
+        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:1024 1031:2048 2055:3072 3079:4096 4103:5120 5127:6144 6151:7168 7175:8192 8199:9216 9223:10240 10247:11264 11271:12288 12295:13312 13319:14336 14343:15360 15367:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>409</v>
+        <v>379</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>410</v>
+        <v>380</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>58</v>
@@ -10491,19 +10499,19 @@
         <v>23</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>413</v>
+        <v>383</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>411</v>
+        <v>381</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>412</v>
+        <v>382</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>414</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -10534,8 +10542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6340C06B-693A-1B48-9921-F23546F2EC49}">
   <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10604,20 +10612,20 @@
     </row>
     <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D2" s="1">
         <v>12.99</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>249</v>
+        <v>430</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -10633,16 +10641,16 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D3" s="1">
         <v>12.99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>354</v>
+        <v>431</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -10656,10 +10664,10 @@
     </row>
     <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>318</v>
+        <v>304</v>
       </c>
       <c r="D4" s="18">
         <v>2.99</v>
@@ -10669,7 +10677,7 @@
     </row>
     <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="C5" s="18" t="s">
-        <v>326</v>
+        <v>312</v>
       </c>
       <c r="D5" s="18">
         <v>2.99</v>
@@ -10690,8 +10698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F85CC15-573B-5848-A683-9CAAED797647}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -10701,7 +10709,7 @@
     <col min="3" max="3" width="25.5" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="1"/>
     <col min="5" max="5" width="44.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.83203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="19" style="1" customWidth="1"/>
     <col min="10" max="10" width="27.6640625" style="1" customWidth="1"/>
@@ -10773,7 +10781,7 @@
         <v>177</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>178</v>
+        <v>432</v>
       </c>
       <c r="I2" s="12"/>
       <c r="J2" s="12"/>
@@ -10785,20 +10793,20 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>328</v>
+        <v>314</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
       <c r="D3" s="1">
         <v>8.99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>331</v>
+        <v>317</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>179</v>
+        <v>434</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -10813,7 +10821,7 @@
       <c r="B4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2" t="s">
-        <v>332</v>
+        <v>318</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>92</v>
@@ -10822,87 +10830,87 @@
         <v>90</v>
       </c>
       <c r="M4" s="2" t="s">
-        <v>333</v>
+        <v>319</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>334</v>
+        <v>320</v>
       </c>
       <c r="O4" s="2"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>327</v>
+        <v>313</v>
       </c>
       <c r="D5" s="1">
         <v>8.99</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>247</v>
+        <v>433</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>329</v>
+        <v>315</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D6" s="1">
         <v>10.99</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>249</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="D7" s="1">
         <v>6.99</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="1" t="s">
-        <v>322</v>
+        <v>308</v>
       </c>
       <c r="D8" s="1">
         <v>6.99</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>323</v>
+        <v>309</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>335</v>
+        <v>321</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>336</v>
+        <v>322</v>
       </c>
       <c r="D9" s="1">
         <v>5.99</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>337</v>
+        <v>323</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>338</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -11350,7 +11358,7 @@
         <v>134</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I14" s="6" t="s">
         <v>131</v>
@@ -11578,7 +11586,7 @@
         <v>87</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="I32" s="6" t="s">
         <v>110</v>
@@ -11586,10 +11594,10 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>157</v>
@@ -11597,7 +11605,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C34" s="6" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>157</v>
@@ -11608,7 +11616,7 @@
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>157</v>
@@ -11616,7 +11624,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C36" s="6" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>157</v>
@@ -11624,10 +11632,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C37" s="6" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>139</v>
@@ -11635,10 +11643,10 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C38" s="6" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="F38" s="6" t="s">
         <v>139</v>
@@ -11646,29 +11654,29 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C39" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G39" s="6" t="s">
         <v>225</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C40" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>157</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C41" s="6" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>157</v>
@@ -11676,27 +11684,27 @@
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C42" s="6" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C43" s="6" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>139</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="J43" s="6" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="K43" s="6" t="s">
         <v>90</v>
@@ -11705,7 +11713,7 @@
         <v>90</v>
       </c>
       <c r="M43" s="6" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="N43" s="6" t="s">
         <v>92</v>
@@ -11713,7 +11721,7 @@
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M44" s="6" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
       <c r="N44" s="6" t="s">
         <v>92</v>
@@ -11721,7 +11729,7 @@
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M45" s="6" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="N45" s="6" t="s">
         <v>92</v>
@@ -11729,10 +11737,10 @@
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I46" s="6" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="J46" s="6" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="K46" s="6" t="s">
         <v>92</v>
@@ -11741,7 +11749,7 @@
         <v>111</v>
       </c>
       <c r="M46" s="6" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="N46" s="6" t="s">
         <v>90</v>
@@ -11749,7 +11757,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M47" s="6" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="N47" s="6" t="s">
         <v>90</v>
@@ -11757,7 +11765,7 @@
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M48" s="6" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="N48" s="6" t="s">
         <v>90</v>
@@ -11765,7 +11773,7 @@
     </row>
     <row r="49" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M49" s="6" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="N49" s="6" t="s">
         <v>90</v>
@@ -11773,7 +11781,7 @@
     </row>
     <row r="50" spans="13:14" x14ac:dyDescent="0.25">
       <c r="M50" s="6" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="N50" s="6" t="s">
         <v>90</v>
@@ -11793,15 +11801,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55EDE47-5436-0749-AB83-3D55441C0ECC}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView topLeftCell="C1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="36.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="113.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11854,39 +11862,39 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>415</v>
+        <v>385</v>
       </c>
       <c r="C2" t="s">
-        <v>417</v>
+        <v>387</v>
       </c>
       <c r="D2">
         <v>7.99</v>
       </c>
       <c r="E2" t="s">
-        <v>419</v>
+        <v>389</v>
       </c>
       <c r="F2" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
       <c r="C3" t="s">
-        <v>420</v>
+        <v>390</v>
       </c>
       <c r="D3">
         <v>9.99</v>
       </c>
       <c r="E3" t="s">
-        <v>423</v>
+        <v>392</v>
       </c>
       <c r="F3" t="s">
-        <v>422</v>
+        <v>401</v>
       </c>
       <c r="J3" t="s">
-        <v>421</v>
+        <v>391</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -11903,50 +11911,53 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>416</v>
+        <v>386</v>
       </c>
       <c r="C4" t="s">
-        <v>424</v>
+        <v>393</v>
       </c>
       <c r="D4">
         <v>11.99</v>
       </c>
       <c r="E4" t="s">
-        <v>426</v>
+        <v>394</v>
       </c>
       <c r="F4" t="s">
-        <v>425</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C5" t="s">
-        <v>427</v>
+        <v>395</v>
       </c>
       <c r="D5">
         <v>4.99</v>
       </c>
       <c r="E5" t="s">
-        <v>428</v>
+        <v>396</v>
       </c>
       <c r="F5" t="s">
-        <v>429</v>
+        <v>399</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C6" t="s">
-        <v>430</v>
+        <v>397</v>
       </c>
       <c r="D6">
         <v>6.99</v>
       </c>
       <c r="E6" t="s">
-        <v>431</v>
+        <v>398</v>
+      </c>
+      <c r="F6" t="s">
+        <v>403</v>
       </c>
     </row>
   </sheetData>
@@ -11960,7 +11971,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11970,7 +11981,7 @@
     <col min="3" max="3" width="30.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" customWidth="1"/>
     <col min="7" max="7" width="11.5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
@@ -12031,58 +12042,61 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>402</v>
+        <v>372</v>
       </c>
       <c r="C2" t="s">
-        <v>403</v>
+        <v>373</v>
       </c>
       <c r="D2">
         <v>14.89</v>
       </c>
       <c r="E2" t="s">
-        <v>402</v>
+        <v>372</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C3" t="s">
-        <v>404</v>
+        <v>374</v>
       </c>
       <c r="D3">
         <v>2.99</v>
       </c>
       <c r="E3" t="s">
+        <v>375</v>
+      </c>
+      <c r="F3" t="s">
         <v>405</v>
-      </c>
-      <c r="F3" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C4" t="s">
-        <v>400</v>
+        <v>370</v>
       </c>
       <c r="D4">
         <v>3.89</v>
       </c>
       <c r="E4" t="s">
-        <v>401</v>
+        <v>371</v>
+      </c>
+      <c r="F4" t="s">
+        <v>402</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>407</v>
+        <v>377</v>
       </c>
       <c r="D5">
         <v>3.89</v>
       </c>
       <c r="E5" t="s">
-        <v>408</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -12095,8 +12109,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BA9BBD-C9D6-C645-B88A-4290D24E034A}">
   <dimension ref="A1:O8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12105,6 +12119,7 @@
     <col min="3" max="3" width="48.33203125" customWidth="1"/>
     <col min="5" max="5" width="58.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="27.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
@@ -12156,109 +12171,109 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>309</v>
+        <v>295</v>
       </c>
       <c r="C2" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="D2">
         <v>10.99</v>
       </c>
       <c r="E2" t="s">
-        <v>307</v>
+        <v>293</v>
       </c>
       <c r="F2" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>308</v>
+        <v>294</v>
       </c>
       <c r="D3">
         <v>10.99</v>
       </c>
       <c r="E3" t="s">
-        <v>306</v>
+        <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>366</v>
+        <v>408</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="D4">
         <v>11.99</v>
       </c>
       <c r="E4" t="s">
-        <v>311</v>
+        <v>297</v>
       </c>
       <c r="F4" t="s">
-        <v>364</v>
+        <v>406</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>312</v>
+        <v>298</v>
       </c>
       <c r="D5">
         <v>11.99</v>
       </c>
       <c r="E5" t="s">
-        <v>313</v>
+        <v>299</v>
       </c>
       <c r="F5" t="s">
-        <v>365</v>
+        <v>407</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>314</v>
+        <v>300</v>
       </c>
       <c r="D6">
         <v>10.99</v>
       </c>
       <c r="E6" t="s">
-        <v>315</v>
+        <v>301</v>
       </c>
       <c r="F6" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>317</v>
+        <v>303</v>
       </c>
       <c r="D7">
         <v>10.99</v>
       </c>
       <c r="E7" t="s">
-        <v>316</v>
+        <v>302</v>
       </c>
       <c r="F7" t="s">
-        <v>366</v>
+        <v>388</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>319</v>
+        <v>305</v>
       </c>
       <c r="C8" t="s">
-        <v>320</v>
+        <v>306</v>
       </c>
       <c r="D8">
         <v>16.989999999999998</v>
       </c>
       <c r="E8" t="s">
-        <v>321</v>
+        <v>307</v>
       </c>
       <c r="F8" t="s">
-        <v>366</v>
+        <v>404</v>
       </c>
       <c r="G8" t="s">
-        <v>325</v>
+        <v>311</v>
       </c>
     </row>
   </sheetData>
@@ -12271,8 +12286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED334EF-9868-4A4E-84D0-B4BC990B1FD4}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12281,7 +12296,7 @@
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="38.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.83203125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="27.6640625" customWidth="1"/>
@@ -12341,20 +12356,20 @@
     </row>
     <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D2" s="1">
         <v>14.95</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>361</v>
+        <v>376</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -12368,20 +12383,20 @@
     </row>
     <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>291</v>
+        <v>277</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D3" s="1">
         <v>16.95</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>362</v>
+        <v>409</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -12395,7 +12410,7 @@
     </row>
     <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>173</v>
@@ -12404,41 +12419,41 @@
         <v>18.95</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>266</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>324</v>
+        <v>310</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>267</v>
+        <v>253</v>
       </c>
       <c r="D5" s="1">
         <v>18.95</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>268</v>
+        <v>254</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>363</v>
+        <v>410</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>269</v>
+        <v>255</v>
       </c>
       <c r="D6" s="1">
         <v>18.95</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>270</v>
+        <v>256</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>363</v>
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -12454,8 +12469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211D9A52-2D82-F545-B3C8-1BEA579932AE}">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -12464,8 +12479,8 @@
     <col min="2" max="2" width="16.1640625" style="19" customWidth="1"/>
     <col min="3" max="3" width="57.1640625" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="19"/>
-    <col min="5" max="5" width="77" style="19" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.33203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="87" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39" style="19" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="144.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.83203125" style="19" customWidth="1"/>
     <col min="9" max="9" width="19" style="19" customWidth="1"/>
@@ -12527,20 +12542,20 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D2" s="1">
         <v>10.99</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -12556,16 +12571,16 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="D3" s="1">
         <v>10.99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>196</v>
+        <v>413</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -12579,59 +12594,61 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="D4" s="1">
         <v>10.99</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="F4" s="1"/>
+        <v>193</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
       <c r="D5" s="1">
         <v>10.99</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>275</v>
+        <v>261</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>280</v>
+        <v>266</v>
       </c>
       <c r="D6" s="1">
         <v>8.99</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>281</v>
+        <v>267</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>367</v>
+        <v>338</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>368</v>
+        <v>339</v>
       </c>
       <c r="D7" s="19">
         <v>9.99</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>175</v>
@@ -12639,162 +12656,164 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="19" t="s">
-        <v>370</v>
+        <v>341</v>
       </c>
       <c r="D8" s="19">
         <v>4.99</v>
       </c>
       <c r="E8" s="19" t="s">
-        <v>371</v>
+        <v>342</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>372</v>
+        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="19" t="s">
-        <v>373</v>
+        <v>344</v>
       </c>
       <c r="D9" s="19">
         <v>9.99</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>374</v>
+        <v>345</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>375</v>
+        <v>417</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>277</v>
+        <v>263</v>
       </c>
       <c r="D10" s="1">
         <v>5.99</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>279</v>
+        <v>265</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>278</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="19" t="s">
-        <v>376</v>
+        <v>346</v>
       </c>
       <c r="D11" s="19">
         <v>2.99</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>381</v>
+        <v>351</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>377</v>
+        <v>347</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="19" t="s">
-        <v>378</v>
+        <v>348</v>
       </c>
       <c r="D12" s="19">
         <v>2.99</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>380</v>
+        <v>350</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>379</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="19" t="s">
-        <v>382</v>
+        <v>352</v>
       </c>
       <c r="D13" s="19">
         <v>2.99</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>383</v>
+        <v>353</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>379</v>
+        <v>349</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="D14" s="1">
         <v>4.99</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>286</v>
+        <v>272</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C15" s="1" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="D15" s="1">
         <v>3.99</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C16" s="1" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="D16" s="1">
         <v>4.99</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>342</v>
+        <v>328</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>339</v>
+        <v>325</v>
       </c>
       <c r="D17" s="1">
         <v>4.99</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>326</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>341</v>
+        <v>327</v>
       </c>
       <c r="D18" s="1">
         <v>3.99</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="19" t="s">
-        <v>343</v>
+        <v>329</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>345</v>
+        <v>331</v>
       </c>
       <c r="K18" s="19">
         <v>0</v>
@@ -12803,13 +12822,13 @@
         <v>1</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>346</v>
+        <v>332</v>
       </c>
       <c r="N18" s="19">
         <v>0</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="3:15" x14ac:dyDescent="0.25">
@@ -12818,13 +12837,13 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="M19" s="19" t="s">
-        <v>347</v>
+        <v>333</v>
       </c>
       <c r="N19" s="19">
         <v>0</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>348</v>
+        <v>412</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
@@ -12833,13 +12852,13 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="M20" s="19" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="N20" s="19">
         <v>0</v>
       </c>
       <c r="O20" s="19" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
@@ -12848,13 +12867,13 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="M21" s="19" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="N21" s="19">
         <v>0</v>
       </c>
       <c r="O21" s="19" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
     </row>
     <row r="22" spans="3:15" x14ac:dyDescent="0.25">
@@ -12863,13 +12882,13 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="M22" s="19" t="s">
-        <v>352</v>
+        <v>414</v>
       </c>
       <c r="N22" s="19">
         <v>0</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>352</v>
+        <v>414</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
@@ -12878,13 +12897,13 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="M23" s="19" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
       <c r="N23" s="19">
         <v>0</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>384</v>
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -12901,7 +12920,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12970,20 +12989,20 @@
     </row>
     <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>292</v>
+        <v>278</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D2" s="15">
         <v>15.99</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>359</v>
+        <v>418</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -12997,31 +13016,31 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>273</v>
+        <v>259</v>
       </c>
       <c r="F3" t="s">
-        <v>358</v>
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B4" s="12"/>
       <c r="C4" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D4" s="15">
         <v>23.99</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F4" s="17"/>
       <c r="G4" s="12"/>
@@ -13036,19 +13055,19 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>294</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
-        <v>272</v>
+        <v>258</v>
       </c>
       <c r="D5">
         <v>7.99</v>
       </c>
       <c r="E5" t="s">
-        <v>274</v>
+        <v>260</v>
       </c>
       <c r="F5" t="s">
-        <v>360</v>
+        <v>388</v>
       </c>
     </row>
   </sheetData>
@@ -13064,8 +13083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6800E-0FE0-C849-BEB9-3BC5DE080FB9}">
   <dimension ref="A1:O4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13073,8 +13092,8 @@
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
     <col min="2" max="2" width="16.1640625" customWidth="1"/>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="44.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="34.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="50.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.83203125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="27.6640625" customWidth="1"/>
@@ -13134,20 +13153,20 @@
     </row>
     <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
-        <v>293</v>
+        <v>279</v>
       </c>
       <c r="B2" s="12"/>
       <c r="C2" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D2" s="15">
         <v>15.99</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>186</v>
+        <v>420</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -13163,16 +13182,16 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D3" s="15">
         <v>13.99</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>189</v>
+        <v>421</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -13186,19 +13205,19 @@
     </row>
     <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>295</v>
+        <v>281</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D4" s="15">
         <v>4.99</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>357</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -13214,8 +13233,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FC3867-0998-7042-A866-D535493EA32D}">
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13225,7 +13244,7 @@
     <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13.83203125" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="27.6640625" customWidth="1"/>
@@ -13287,16 +13306,16 @@
       <c r="A2" s="12"/>
       <c r="B2" s="12"/>
       <c r="C2" s="1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D2" s="1">
         <v>10.99</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>205</v>
+        <v>422</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -13312,16 +13331,16 @@
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="1" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="D3" s="1">
         <v>14.99</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>208</v>
+        <v>429</v>
       </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -13335,88 +13354,88 @@
     </row>
     <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
       <c r="D4" s="1">
         <v>14.99</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>211</v>
+        <v>423</v>
       </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D5">
         <v>13.99</v>
       </c>
       <c r="E5" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="F5" t="s">
-        <v>356</v>
+        <v>424</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D6">
         <v>12.99</v>
       </c>
       <c r="E6" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="F6" t="s">
-        <v>255</v>
+        <v>425</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D7">
         <v>17.989999999999998</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="F7" t="s">
-        <v>355</v>
+        <v>428</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
       <c r="D8">
         <v>14.99</v>
       </c>
       <c r="E8" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
       <c r="F8" t="s">
-        <v>261</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D9">
         <v>10.99</v>
       </c>
       <c r="E9" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
       <c r="F9" t="s">
-        <v>264</v>
+        <v>426</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
allergen modification (not finished)
</commit_message>
<xml_diff>
--- a/Backend/database/restaurants_menus.xlsx
+++ b/Backend/database/restaurants_menus.xlsx
@@ -1,31 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/erin/Desktop/Senior Proj/Backend/database/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunaukawa/GitHub/CS417SRProject/Backend/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E33A45E-4551-E84A-856E-7A47300CBCB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10482015-C0D7-6444-8A6D-A01C206968F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25080" windowHeight="18000" activeTab="10" xr2:uid="{3E180D32-923C-C640-8E37-FF46F6D4E035}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25080" windowHeight="17500" xr2:uid="{3E180D32-923C-C640-8E37-FF46F6D4E035}"/>
   </bookViews>
   <sheets>
-    <sheet name="restaurants" sheetId="1" r:id="rId1"/>
-    <sheet name="panera" sheetId="13" r:id="rId2"/>
-    <sheet name="nandos" sheetId="12" r:id="rId3"/>
-    <sheet name="cheesecake_factory" sheetId="11" r:id="rId4"/>
-    <sheet name="gusto_trattoria" sheetId="10" r:id="rId5"/>
-    <sheet name="pret_a_manger" sheetId="9" r:id="rId6"/>
-    <sheet name="texas_roadhouse" sheetId="8" r:id="rId7"/>
-    <sheet name="bonchon" sheetId="7" r:id="rId8"/>
-    <sheet name="mecha" sheetId="6" r:id="rId9"/>
-    <sheet name="colony_grill" sheetId="5" r:id="rId10"/>
-    <sheet name="lindas" sheetId="4" r:id="rId11"/>
-    <sheet name="63s" sheetId="3" r:id="rId12"/>
-    <sheet name="jps" sheetId="2" r:id="rId13"/>
+    <sheet name="allergens" sheetId="14" r:id="rId1"/>
+    <sheet name="restaurants" sheetId="1" r:id="rId2"/>
+    <sheet name="panera" sheetId="13" r:id="rId3"/>
+    <sheet name="nandos" sheetId="12" r:id="rId4"/>
+    <sheet name="cheesecake_factory" sheetId="11" r:id="rId5"/>
+    <sheet name="gusto_trattoria" sheetId="10" r:id="rId6"/>
+    <sheet name="pret_a_manger" sheetId="9" r:id="rId7"/>
+    <sheet name="texas_roadhouse" sheetId="8" r:id="rId8"/>
+    <sheet name="bonchon" sheetId="7" r:id="rId9"/>
+    <sheet name="mecha" sheetId="6" r:id="rId10"/>
+    <sheet name="colony_grill" sheetId="5" r:id="rId11"/>
+    <sheet name="lindas" sheetId="4" r:id="rId12"/>
+    <sheet name="63s" sheetId="3" r:id="rId13"/>
+    <sheet name="jps" sheetId="2" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1914,7 +1915,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="452">
   <si>
     <t>name</t>
   </si>
@@ -2888,9 +2889,6 @@
     <t>Cheese, Bread</t>
   </si>
   <si>
-    <t>Wheat, Dairy</t>
-  </si>
-  <si>
     <t>Strawberry Lavender Black Tea</t>
   </si>
   <si>
@@ -3185,9 +3183,6 @@
     <t>Fish, Soybeans, Wheat, Sesame, Pine Nuts</t>
   </si>
   <si>
-    <t>Egg, Sesame, Soybeans, Wheat</t>
-  </si>
-  <si>
     <t>Milk, Sesame, Soybeans, Wheat</t>
   </si>
   <si>
@@ -3215,10 +3210,67 @@
     <t>Fish, Wheat, Crab</t>
   </si>
   <si>
-    <t>Wheat, Egg, Milk</t>
-  </si>
-  <si>
     <t>Wheat, Milk, Soybeans, Eggs</t>
+  </si>
+  <si>
+    <t>Eggs, Sesame, Soybeans, Wheat</t>
+  </si>
+  <si>
+    <t>allergen_group</t>
+  </si>
+  <si>
+    <t>other_names</t>
+  </si>
+  <si>
+    <t>allergen</t>
+  </si>
+  <si>
+    <t>Dairy</t>
+  </si>
+  <si>
+    <t>Crustacean Shellfish</t>
+  </si>
+  <si>
+    <t>Shellfish</t>
+  </si>
+  <si>
+    <t>Peanuts</t>
+  </si>
+  <si>
+    <t>Tree Nuts</t>
+  </si>
+  <si>
+    <t>Soy</t>
+  </si>
+  <si>
+    <t>Gluten</t>
+  </si>
+  <si>
+    <t>Sesame</t>
+  </si>
+  <si>
+    <t>Mustard</t>
+  </si>
+  <si>
+    <t>Celery</t>
+  </si>
+  <si>
+    <t>Garlic</t>
+  </si>
+  <si>
+    <t>Buckwheat</t>
+  </si>
+  <si>
+    <t>Tilapia, Salmon, Cod, Trout, Tuna, Anchovy</t>
+  </si>
+  <si>
+    <t>Shrimp, Crab, Lobster</t>
+  </si>
+  <si>
+    <t>Almonds, Brazil Nuts, Cashews, Chestnuts, Hazelnuts, Macadamia Nuts, Pecans, Pistachios, Walnuts, Pine Nuts</t>
+  </si>
+  <si>
+    <t>Apple, Avocado, Banana, Cherry, Kiwi, Melon, Peach, Pear, Pinapple, Plum, Strawberry, Watermelon</t>
   </si>
 </sst>
 </file>
@@ -5205,6 +5257,58 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{231BBEA5-5CCB-2346-B8C0-71972FA906CF}" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
+  <autoFilter ref="A1:C16" xr:uid="{231BBEA5-5CCB-2346-B8C0-71972FA906CF}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{6EF2395E-DC6F-3C4F-BF92-3BF424C26F3A}" name="allergen_group"/>
+    <tableColumn id="2" xr3:uid="{54AEB0A5-B5A4-3044-B0C9-524DD74B40EB}" name="other_names"/>
+    <tableColumn id="3" xr3:uid="{707FEDC5-9858-F64B-B63B-19F289BCEE4E}" name="allergen"/>
+  </tableColumns>
+  <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}" name="Table5" displayName="Table5" ref="A1:O50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O50" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{1853C437-6A62-6B47-8C9B-564DEA57939A}" name="category" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7CC90834-B0D1-C849-9B51-B5D9EA77DAA0}" name="sub_category" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{5FF08993-59DB-6349-A6EA-32533F571FF5}" name="name" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{7CF1E11B-4F70-B44E-872E-BCCD8BFE7D9D}" name="price" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{3BF4A478-AEA5-7A41-B357-48C9836E1C80}" name="ingredients" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{E2E7B27E-AAA8-514A-8148-667D740D3AA7}" name="allergens" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{B1097D52-302C-544C-A429-413DED807F5F}" name="description" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{1F2AE8F3-03BD-7B45-A4C7-02179D959056}" name="image_filename" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{49269410-C082-8540-AD51-99931EBA2F5B}" name="option_group_id" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{B8E445A1-F5E1-5047-A344-69C841DD833C}" name="option_group_description" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{21396A92-76A0-2442-B8F3-1DA062E205CC}" name="option_min_quantity" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{557EC8C7-A1C9-F84C-B74C-2B1F02DFEF2A}" name="option_max_quantity" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{E71702D2-99DB-F44C-9D2F-810A07ED5309}" name="option_item_name" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{955FD788-14F2-AA4C-B201-A840E08AD65B}" name="extra_price" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{23C3A0BD-31DD-7249-B139-0E6149C8E21D}" name="option_allergens" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{449F4F08-14A7-854B-A85B-E93306BD0212}" name="Table2" displayName="Table2" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
   <autoFilter ref="A1:Q14" xr:uid="{449F4F08-14A7-854B-A85B-E93306BD0212}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5248,7 +5352,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{DAC74174-4265-A84F-8FE7-21CD54220646}" name="Table16" displayName="Table16" ref="A1:O6" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75">
   <autoFilter ref="A1:O6" xr:uid="{DAC74174-4265-A84F-8FE7-21CD54220646}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5288,7 +5392,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{9891CE72-5244-1547-9248-A1EF2B8A5D67}" name="Table15" displayName="Table15" ref="A1:O23" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67">
   <autoFilter ref="A1:O23" xr:uid="{9891CE72-5244-1547-9248-A1EF2B8A5D67}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5328,7 +5432,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AFB4B9C8-896F-2B4C-9AEC-68AD2E00C8C0}" name="Table14" displayName="Table14" ref="A1:O5" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A1:O5" xr:uid="{AFB4B9C8-896F-2B4C-9AEC-68AD2E00C8C0}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5368,7 +5472,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7F42674C-F8E2-BD46-B0CD-6C935E6CF276}" name="Table13" displayName="Table13" ref="A1:O4" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46">
   <autoFilter ref="A1:O4" xr:uid="{7F42674C-F8E2-BD46-B0CD-6C935E6CF276}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5408,7 +5512,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{53A31204-2F15-774A-9217-6321151D9A7C}" name="Table12" displayName="Table12" ref="A1:O9" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A1:O9" xr:uid="{53A31204-2F15-774A-9217-6321151D9A7C}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5448,7 +5552,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{889E6C16-6078-5B43-9A22-05E9C269B41C}" name="Table11" displayName="Table11" ref="A1:O5" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A1:O5" xr:uid="{889E6C16-6078-5B43-9A22-05E9C269B41C}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5488,7 +5592,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{2B8457F3-C4FB-F848-A16E-EF50D38EF95F}" name="Table10" displayName="Table10" ref="A1:O9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32">
   <autoFilter ref="A1:O9" xr:uid="{2B8457F3-C4FB-F848-A16E-EF50D38EF95F}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5523,46 +5627,6 @@
     <tableColumn id="12" xr3:uid="{EB21D867-EC2A-1046-9372-97B5F5F39552}" name="option_item_name" dataDxfId="19"/>
     <tableColumn id="13" xr3:uid="{83CFFF5F-DD2A-6849-B86D-92DB38FF7001}" name="extra_price" dataDxfId="18"/>
     <tableColumn id="14" xr3:uid="{1CFC430A-35A6-3847-A639-DA9CF813A9A8}" name="option_allergens" dataDxfId="17"/>
-  </tableColumns>
-  <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}" name="Table5" displayName="Table5" ref="A1:O50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O50" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-    <filterColumn colId="12" hiddenButton="1"/>
-    <filterColumn colId="13" hiddenButton="1"/>
-    <filterColumn colId="14" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{1853C437-6A62-6B47-8C9B-564DEA57939A}" name="category" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7CC90834-B0D1-C849-9B51-B5D9EA77DAA0}" name="sub_category" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{5FF08993-59DB-6349-A6EA-32533F571FF5}" name="name" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{7CF1E11B-4F70-B44E-872E-BCCD8BFE7D9D}" name="price" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{3BF4A478-AEA5-7A41-B357-48C9836E1C80}" name="ingredients" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{E2E7B27E-AAA8-514A-8148-667D740D3AA7}" name="allergens" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{B1097D52-302C-544C-A429-413DED807F5F}" name="description" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{1F2AE8F3-03BD-7B45-A4C7-02179D959056}" name="image_filename" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{49269410-C082-8540-AD51-99931EBA2F5B}" name="option_group_id" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{B8E445A1-F5E1-5047-A344-69C841DD833C}" name="option_group_description" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{21396A92-76A0-2442-B8F3-1DA062E205CC}" name="option_min_quantity" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{557EC8C7-A1C9-F84C-B74C-2B1F02DFEF2A}" name="option_max_quantity" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{E71702D2-99DB-F44C-9D2F-810A07ED5309}" name="option_item_name" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{955FD788-14F2-AA4C-B201-A840E08AD65B}" name="extra_price" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{23C3A0BD-31DD-7249-B139-0E6149C8E21D}" name="option_allergens" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5884,11 +5948,1625 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67AA6E6-57DF-0445-A312-EF76BC1FF882}">
+  <dimension ref="A1:C16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="11.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>433</v>
+      </c>
+      <c r="B1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>241</v>
+      </c>
+      <c r="B2" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>437</v>
+      </c>
+      <c r="B5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C5" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>440</v>
+      </c>
+      <c r="C6" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>411</v>
+      </c>
+      <c r="B8" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>413</v>
+      </c>
+      <c r="B9" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>402</v>
+      </c>
+      <c r="C11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>353</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FC3867-0998-7042-A866-D535493EA32D}">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10.99</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14.99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="1">
+        <v>14.99</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5">
+        <v>13.99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6">
+        <v>12.99</v>
+      </c>
+      <c r="E6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="E7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F7" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8">
+        <v>14.99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>249</v>
+      </c>
+      <c r="F8" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9">
+        <v>10.99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F9" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6340C06B-693A-1B48-9921-F23546F2EC49}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="18">
+        <v>2.99</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2.99</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F85CC15-573B-5848-A683-9CAAED797647}">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="44.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10.99</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA28EF5A-AAA6-E243-A364-89A6CC876E03}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B315ED-1831-0A4D-AF4E-5349EB3E43E8}">
+  <dimension ref="A1:O50"/>
+  <sheetViews>
+    <sheetView topLeftCell="G6" zoomScale="103" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="6"/>
+    <col min="2" max="2" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.5" style="6"/>
+    <col min="7" max="7" width="63.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="6"/>
+    <col min="9" max="9" width="27.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" style="6" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="6"/>
+    <col min="14" max="14" width="19.1640625" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="14.5" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="M6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="M7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="M8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="M10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I18" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M21" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I23" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M25" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M26" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M28" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C36" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C37" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C38" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C39" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C40" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C41" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C42" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C43" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M44" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I46" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M47" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M48" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M50" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4635569-6B50-5940-8C00-E7257ADB0B0E}">
   <dimension ref="A1:XFD14"/>
   <sheetViews>
     <sheetView zoomScale="92" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -10190,25 +11868,25 @@
         <v>124</v>
       </c>
       <c r="K5" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="O5" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="L5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="M5" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="O5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>356</v>
-      </c>
-      <c r="P5" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:1024 1031:2048 2055:3072 3079:4096 4103:5120 5127:6144 6151:7168 7175:8192 8199:9216 9223:10240 10247:11264 11271:12288 12295:13312 13319:14336 14343:15360 15367:16384" x14ac:dyDescent="0.25">
@@ -10414,16 +12092,16 @@
         <v>2033717205</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="O12" s="6" t="s">
         <v>289</v>
@@ -10437,60 +12115,60 @@
     </row>
     <row r="13" spans="1:1024 1031:2048 2055:3072 3079:4096 4103:5120 5127:6144 6151:7168 7175:8192 8199:9216 9223:10240 10247:11264 11271:12288 12295:13312 13319:14336 14343:15360 15367:16384" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="6" t="s">
         <v>359</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>360</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>43</v>
       </c>
       <c r="E13" s="21" t="s">
+        <v>360</v>
+      </c>
+      <c r="F13" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="F13" s="6" t="s">
-        <v>362</v>
-      </c>
       <c r="G13" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>368</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>369</v>
       </c>
       <c r="I13">
         <v>3016868388</v>
       </c>
       <c r="K13" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M13" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="N13" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="O13" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="N13" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="O13" s="6" t="s">
+      <c r="P13" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q13" s="6" t="s">
         <v>366</v>
-      </c>
-      <c r="P13" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="Q13" s="6" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="14" spans="1:1024 1031:2048 2055:3072 3079:4096 4103:5120 5127:6144 6151:7168 7175:8192 8199:9216 9223:10240 10247:11264 11271:12288 12295:13312 13319:14336 14343:15360 15367:16384" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
+        <v>378</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>379</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>380</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>58</v>
@@ -10499,19 +12177,19 @@
         <v>23</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="H14" s="6" t="s">
-        <v>382</v>
-      </c>
       <c r="I14" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -10538,1266 +12216,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6340C06B-693A-1B48-9921-F23546F2EC49}">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D2" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D3" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>270</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="D4" s="18">
-        <v>2.99</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="D5" s="18">
-        <v>2.99</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F85CC15-573B-5848-A683-9CAAED797647}">
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="44.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="1">
-        <v>9.99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8.99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D5" s="1">
-        <v>8.99</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="1">
-        <v>10.99</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>430</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D8" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="D9" s="1">
-        <v>5.99</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>324</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA28EF5A-AAA6-E243-A364-89A6CC876E03}">
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B315ED-1831-0A4D-AF4E-5349EB3E43E8}">
-  <dimension ref="A1:O50"/>
-  <sheetViews>
-    <sheetView topLeftCell="G6" zoomScale="103" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5" style="6"/>
-    <col min="2" max="2" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.5" style="6"/>
-    <col min="7" max="7" width="63.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="6"/>
-    <col min="9" max="9" width="27.6640625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="6" customWidth="1"/>
-    <col min="13" max="13" width="14.5" style="6"/>
-    <col min="14" max="14" width="19.1640625" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="14.5" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M3" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="M6" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="M7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="M8" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="M10" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M15" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M16" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M17" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I18" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I19" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M20" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M21" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M22" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I23" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I24" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M25" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M26" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M27" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M28" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I29" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M30" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M31" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C34" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C37" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C39" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C40" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C41" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C42" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C43" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M44" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M45" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I46" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="M46" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="N46" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M47" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M48" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M49" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="N49" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M50" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="N50" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55EDE47-5436-0749-AB83-3D55441C0ECC}">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -11862,39 +12281,39 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C2" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D2">
         <v>7.99</v>
       </c>
       <c r="E2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="F2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D3">
         <v>9.99</v>
       </c>
       <c r="E3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="F3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="J3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K3">
         <v>0</v>
@@ -11911,19 +12330,19 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C4" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D4">
         <v>11.99</v>
       </c>
       <c r="E4" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="F4" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -11931,16 +12350,16 @@
         <v>269</v>
       </c>
       <c r="C5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D5">
         <v>4.99</v>
       </c>
       <c r="E5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="F5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -11948,16 +12367,16 @@
         <v>270</v>
       </c>
       <c r="C6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D6">
         <v>6.99</v>
       </c>
       <c r="E6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="F6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
   </sheetData>
@@ -11966,7 +12385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C84630-6BE4-A64D-87E5-C7ECC341418B}">
   <dimension ref="A1:O5"/>
   <sheetViews>
@@ -12042,16 +12461,16 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>371</v>
+      </c>
+      <c r="C2" t="s">
         <v>372</v>
-      </c>
-      <c r="C2" t="s">
-        <v>373</v>
       </c>
       <c r="D2">
         <v>14.89</v>
       </c>
       <c r="E2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -12059,16 +12478,16 @@
         <v>281</v>
       </c>
       <c r="C3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D3">
         <v>2.99</v>
       </c>
       <c r="E3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="F3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -12076,27 +12495,27 @@
         <v>270</v>
       </c>
       <c r="C4" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D4">
         <v>3.89</v>
       </c>
       <c r="E4" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="F4" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D5">
         <v>3.89</v>
       </c>
       <c r="E5" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
   </sheetData>
@@ -12105,7 +12524,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BA9BBD-C9D6-C645-B88A-4290D24E034A}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -12183,7 +12602,7 @@
         <v>293</v>
       </c>
       <c r="F2" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -12197,7 +12616,7 @@
         <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -12211,7 +12630,7 @@
         <v>297</v>
       </c>
       <c r="F4" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -12225,7 +12644,7 @@
         <v>299</v>
       </c>
       <c r="F5" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -12239,7 +12658,7 @@
         <v>301</v>
       </c>
       <c r="F6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
@@ -12253,7 +12672,7 @@
         <v>302</v>
       </c>
       <c r="F7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
@@ -12270,7 +12689,7 @@
         <v>307</v>
       </c>
       <c r="F8" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="G8" t="s">
         <v>311</v>
@@ -12282,7 +12701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED334EF-9868-4A4E-84D0-B4BC990B1FD4}">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -12369,7 +12788,7 @@
         <v>195</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -12396,7 +12815,7 @@
         <v>197</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -12422,7 +12841,7 @@
         <v>252</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
@@ -12439,7 +12858,7 @@
         <v>254</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="19" x14ac:dyDescent="0.25">
@@ -12453,7 +12872,7 @@
         <v>256</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
   </sheetData>
@@ -12465,7 +12884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211D9A52-2D82-F545-B3C8-1BEA579932AE}">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -12555,7 +12974,7 @@
         <v>189</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -12580,7 +12999,7 @@
         <v>191</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -12603,7 +13022,7 @@
         <v>193</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -12639,16 +13058,16 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="C7" s="19" t="s">
         <v>338</v>
-      </c>
-      <c r="C7" s="19" t="s">
-        <v>339</v>
       </c>
       <c r="D7" s="19">
         <v>9.99</v>
       </c>
       <c r="E7" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F7" s="19" t="s">
         <v>175</v>
@@ -12656,30 +13075,30 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C8" s="19" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D8" s="19">
         <v>4.99</v>
       </c>
       <c r="E8" s="19" t="s">
+        <v>341</v>
+      </c>
+      <c r="F8" s="19" t="s">
         <v>342</v>
-      </c>
-      <c r="F8" s="19" t="s">
-        <v>343</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C9" s="19" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D9" s="19">
         <v>9.99</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -12701,44 +13120,44 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C11" s="19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D11" s="19">
         <v>2.99</v>
       </c>
       <c r="E11" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C12" s="19" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D12" s="19">
         <v>2.99</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C13" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D13" s="19">
         <v>2.99</v>
       </c>
       <c r="E13" s="19" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -12780,40 +13199,40 @@
         <v>4.99</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D17" s="1">
         <v>4.99</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D18" s="1">
         <v>3.99</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="19" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="K18" s="19">
         <v>0</v>
@@ -12822,7 +13241,7 @@
         <v>1</v>
       </c>
       <c r="M18" s="19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="N18" s="19">
         <v>0</v>
@@ -12837,13 +13256,13 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="M19" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="N19" s="19">
         <v>0</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
@@ -12852,13 +13271,13 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="M20" s="19" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="N20" s="19">
         <v>0</v>
       </c>
       <c r="O20" s="19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="21" spans="3:15" x14ac:dyDescent="0.25">
@@ -12867,7 +13286,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="M21" s="19" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N21" s="19">
         <v>0</v>
@@ -12882,13 +13301,13 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="M22" s="19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="N22" s="19">
         <v>0</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
@@ -12897,13 +13316,13 @@
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
       <c r="M23" s="19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="N23" s="19">
         <v>0</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
   </sheetData>
@@ -12915,7 +13334,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67AC912-884F-F44F-A6CD-51118C2A7D9A}">
   <dimension ref="A1:O5"/>
   <sheetViews>
@@ -13002,7 +13421,7 @@
         <v>181</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -13025,7 +13444,7 @@
         <v>259</v>
       </c>
       <c r="F3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
@@ -13067,7 +13486,7 @@
         <v>260</v>
       </c>
       <c r="F5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
   </sheetData>
@@ -13079,7 +13498,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6800E-0FE0-C849-BEB9-3BC5DE080FB9}">
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -13166,7 +13585,7 @@
         <v>183</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -13191,7 +13610,7 @@
         <v>185</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -13217,225 +13636,7 @@
         <v>187</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>337</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FC3867-0998-7042-A866-D535493EA32D}">
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10.99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>242</v>
-      </c>
-      <c r="D5">
-        <v>13.99</v>
-      </c>
-      <c r="E5" t="s">
-        <v>243</v>
-      </c>
-      <c r="F5" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D6">
-        <v>12.99</v>
-      </c>
-      <c r="E6" t="s">
-        <v>245</v>
-      </c>
-      <c r="F6" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>246</v>
-      </c>
-      <c r="D7">
-        <v>17.989999999999998</v>
-      </c>
-      <c r="E7" t="s">
-        <v>247</v>
-      </c>
-      <c r="F7" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>248</v>
-      </c>
-      <c r="D8">
-        <v>14.99</v>
-      </c>
-      <c r="E8" t="s">
-        <v>249</v>
-      </c>
-      <c r="F8" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>250</v>
-      </c>
-      <c r="D9">
-        <v>10.99</v>
-      </c>
-      <c r="E9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F9" t="s">
-        <v>426</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed allergy filter bugs
</commit_message>
<xml_diff>
--- a/Backend/database/restaurants_menus.xlsx
+++ b/Backend/database/restaurants_menus.xlsx
@@ -8,25 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yunaukawa/GitHub/CS417SRProject/Backend/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10482015-C0D7-6444-8A6D-A01C206968F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2696BA6D-4286-E344-A76F-3544561D637C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25080" windowHeight="17500" xr2:uid="{3E180D32-923C-C640-8E37-FF46F6D4E035}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25080" windowHeight="17500" activeTab="1" xr2:uid="{3E180D32-923C-C640-8E37-FF46F6D4E035}"/>
   </bookViews>
   <sheets>
-    <sheet name="allergens" sheetId="14" r:id="rId1"/>
-    <sheet name="restaurants" sheetId="1" r:id="rId2"/>
-    <sheet name="panera" sheetId="13" r:id="rId3"/>
-    <sheet name="nandos" sheetId="12" r:id="rId4"/>
-    <sheet name="cheesecake_factory" sheetId="11" r:id="rId5"/>
-    <sheet name="gusto_trattoria" sheetId="10" r:id="rId6"/>
-    <sheet name="pret_a_manger" sheetId="9" r:id="rId7"/>
-    <sheet name="texas_roadhouse" sheetId="8" r:id="rId8"/>
-    <sheet name="bonchon" sheetId="7" r:id="rId9"/>
-    <sheet name="mecha" sheetId="6" r:id="rId10"/>
-    <sheet name="colony_grill" sheetId="5" r:id="rId11"/>
-    <sheet name="lindas" sheetId="4" r:id="rId12"/>
-    <sheet name="63s" sheetId="3" r:id="rId13"/>
-    <sheet name="jps" sheetId="2" r:id="rId14"/>
+    <sheet name="restaurants" sheetId="1" r:id="rId1"/>
+    <sheet name="panera" sheetId="13" r:id="rId2"/>
+    <sheet name="nandos" sheetId="12" r:id="rId3"/>
+    <sheet name="cheesecake_factory" sheetId="11" r:id="rId4"/>
+    <sheet name="gusto_trattoria" sheetId="10" r:id="rId5"/>
+    <sheet name="pret_a_manger" sheetId="9" r:id="rId6"/>
+    <sheet name="texas_roadhouse" sheetId="8" r:id="rId7"/>
+    <sheet name="bonchon" sheetId="7" r:id="rId8"/>
+    <sheet name="mecha" sheetId="6" r:id="rId9"/>
+    <sheet name="colony_grill" sheetId="5" r:id="rId10"/>
+    <sheet name="lindas" sheetId="4" r:id="rId11"/>
+    <sheet name="63s" sheetId="3" r:id="rId12"/>
+    <sheet name="jps" sheetId="2" r:id="rId13"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -1915,7 +1914,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="452">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="433">
   <si>
     <t>name</t>
   </si>
@@ -3114,9 +3113,6 @@
     <t>Egg, Milk, Almonds, Wheat, Soybeans</t>
   </si>
   <si>
-    <t>Egg, Walnut, Wheat, Celery</t>
-  </si>
-  <si>
     <t>Milk, Egg, Avocado</t>
   </si>
   <si>
@@ -3216,61 +3212,7 @@
     <t>Eggs, Sesame, Soybeans, Wheat</t>
   </si>
   <si>
-    <t>allergen_group</t>
-  </si>
-  <si>
-    <t>other_names</t>
-  </si>
-  <si>
-    <t>allergen</t>
-  </si>
-  <si>
-    <t>Dairy</t>
-  </si>
-  <si>
-    <t>Crustacean Shellfish</t>
-  </si>
-  <si>
-    <t>Shellfish</t>
-  </si>
-  <si>
-    <t>Peanuts</t>
-  </si>
-  <si>
-    <t>Tree Nuts</t>
-  </si>
-  <si>
-    <t>Soy</t>
-  </si>
-  <si>
-    <t>Gluten</t>
-  </si>
-  <si>
-    <t>Sesame</t>
-  </si>
-  <si>
-    <t>Mustard</t>
-  </si>
-  <si>
-    <t>Celery</t>
-  </si>
-  <si>
-    <t>Garlic</t>
-  </si>
-  <si>
-    <t>Buckwheat</t>
-  </si>
-  <si>
-    <t>Tilapia, Salmon, Cod, Trout, Tuna, Anchovy</t>
-  </si>
-  <si>
-    <t>Shrimp, Crab, Lobster</t>
-  </si>
-  <si>
-    <t>Almonds, Brazil Nuts, Cashews, Chestnuts, Hazelnuts, Macadamia Nuts, Pecans, Pistachios, Walnuts, Pine Nuts</t>
-  </si>
-  <si>
-    <t>Apple, Avocado, Banana, Cherry, Kiwi, Melon, Peach, Pear, Pinapple, Plum, Strawberry, Watermelon</t>
+    <t>Egg, Walnuts, Wheat, Celery</t>
   </si>
 </sst>
 </file>
@@ -5257,58 +5199,6 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{231BBEA5-5CCB-2346-B8C0-71972FA906CF}" name="Table1" displayName="Table1" ref="A1:C16" totalsRowShown="0">
-  <autoFilter ref="A1:C16" xr:uid="{231BBEA5-5CCB-2346-B8C0-71972FA906CF}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{6EF2395E-DC6F-3C4F-BF92-3BF424C26F3A}" name="allergen_group"/>
-    <tableColumn id="2" xr3:uid="{54AEB0A5-B5A4-3044-B0C9-524DD74B40EB}" name="other_names"/>
-    <tableColumn id="3" xr3:uid="{707FEDC5-9858-F64B-B63B-19F289BCEE4E}" name="allergen"/>
-  </tableColumns>
-  <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}" name="Table5" displayName="Table5" ref="A1:O50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A1:O50" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}">
-    <filterColumn colId="0" hiddenButton="1"/>
-    <filterColumn colId="1" hiddenButton="1"/>
-    <filterColumn colId="2" hiddenButton="1"/>
-    <filterColumn colId="3" hiddenButton="1"/>
-    <filterColumn colId="4" hiddenButton="1"/>
-    <filterColumn colId="5" hiddenButton="1"/>
-    <filterColumn colId="6" hiddenButton="1"/>
-    <filterColumn colId="7" hiddenButton="1"/>
-    <filterColumn colId="8" hiddenButton="1"/>
-    <filterColumn colId="9" hiddenButton="1"/>
-    <filterColumn colId="10" hiddenButton="1"/>
-    <filterColumn colId="11" hiddenButton="1"/>
-    <filterColumn colId="12" hiddenButton="1"/>
-    <filterColumn colId="13" hiddenButton="1"/>
-    <filterColumn colId="14" hiddenButton="1"/>
-  </autoFilter>
-  <tableColumns count="15">
-    <tableColumn id="1" xr3:uid="{1853C437-6A62-6B47-8C9B-564DEA57939A}" name="category" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{7CC90834-B0D1-C849-9B51-B5D9EA77DAA0}" name="sub_category" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{5FF08993-59DB-6349-A6EA-32533F571FF5}" name="name" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{7CF1E11B-4F70-B44E-872E-BCCD8BFE7D9D}" name="price" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{3BF4A478-AEA5-7A41-B357-48C9836E1C80}" name="ingredients" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{E2E7B27E-AAA8-514A-8148-667D740D3AA7}" name="allergens" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{B1097D52-302C-544C-A429-413DED807F5F}" name="description" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{1F2AE8F3-03BD-7B45-A4C7-02179D959056}" name="image_filename" dataDxfId="7"/>
-    <tableColumn id="15" xr3:uid="{49269410-C082-8540-AD51-99931EBA2F5B}" name="option_group_id" dataDxfId="6"/>
-    <tableColumn id="8" xr3:uid="{B8E445A1-F5E1-5047-A344-69C841DD833C}" name="option_group_description" dataDxfId="5"/>
-    <tableColumn id="9" xr3:uid="{21396A92-76A0-2442-B8F3-1DA062E205CC}" name="option_min_quantity" dataDxfId="4"/>
-    <tableColumn id="10" xr3:uid="{557EC8C7-A1C9-F84C-B74C-2B1F02DFEF2A}" name="option_max_quantity" dataDxfId="3"/>
-    <tableColumn id="11" xr3:uid="{E71702D2-99DB-F44C-9D2F-810A07ED5309}" name="option_item_name" dataDxfId="2"/>
-    <tableColumn id="12" xr3:uid="{955FD788-14F2-AA4C-B201-A840E08AD65B}" name="extra_price" dataDxfId="1"/>
-    <tableColumn id="13" xr3:uid="{23C3A0BD-31DD-7249-B139-0E6149C8E21D}" name="option_allergens" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
-</file>
-
-<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{449F4F08-14A7-854B-A85B-E93306BD0212}" name="Table2" displayName="Table2" ref="A1:Q14" totalsRowShown="0" headerRowDxfId="96" dataDxfId="95">
   <autoFilter ref="A1:Q14" xr:uid="{449F4F08-14A7-854B-A85B-E93306BD0212}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5352,7 +5242,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{DAC74174-4265-A84F-8FE7-21CD54220646}" name="Table16" displayName="Table16" ref="A1:O6" totalsRowShown="0" headerRowDxfId="77" headerRowBorderDxfId="76" tableBorderDxfId="75">
   <autoFilter ref="A1:O6" xr:uid="{DAC74174-4265-A84F-8FE7-21CD54220646}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5392,7 +5282,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{9891CE72-5244-1547-9248-A1EF2B8A5D67}" name="Table15" displayName="Table15" ref="A1:O23" totalsRowShown="0" headerRowDxfId="70" dataDxfId="68" headerRowBorderDxfId="69" tableBorderDxfId="67">
   <autoFilter ref="A1:O23" xr:uid="{9891CE72-5244-1547-9248-A1EF2B8A5D67}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5432,7 +5322,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AFB4B9C8-896F-2B4C-9AEC-68AD2E00C8C0}" name="Table14" displayName="Table14" ref="A1:O5" totalsRowShown="0" headerRowDxfId="51" headerRowBorderDxfId="50" tableBorderDxfId="49">
   <autoFilter ref="A1:O5" xr:uid="{AFB4B9C8-896F-2B4C-9AEC-68AD2E00C8C0}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5472,7 +5362,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{7F42674C-F8E2-BD46-B0CD-6C935E6CF276}" name="Table13" displayName="Table13" ref="A1:O4" totalsRowShown="0" headerRowDxfId="48" headerRowBorderDxfId="47" tableBorderDxfId="46">
   <autoFilter ref="A1:O4" xr:uid="{7F42674C-F8E2-BD46-B0CD-6C935E6CF276}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5512,7 +5402,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{53A31204-2F15-774A-9217-6321151D9A7C}" name="Table12" displayName="Table12" ref="A1:O9" totalsRowShown="0" headerRowDxfId="45" headerRowBorderDxfId="44" tableBorderDxfId="43">
   <autoFilter ref="A1:O9" xr:uid="{53A31204-2F15-774A-9217-6321151D9A7C}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5552,7 +5442,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{889E6C16-6078-5B43-9A22-05E9C269B41C}" name="Table11" displayName="Table11" ref="A1:O5" totalsRowShown="0" headerRowDxfId="42" headerRowBorderDxfId="41" tableBorderDxfId="40">
   <autoFilter ref="A1:O5" xr:uid="{889E6C16-6078-5B43-9A22-05E9C269B41C}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5592,7 +5482,7 @@
 </table>
 </file>
 
-<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{2B8457F3-C4FB-F848-A16E-EF50D38EF95F}" name="Table10" displayName="Table10" ref="A1:O9" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32">
   <autoFilter ref="A1:O9" xr:uid="{2B8457F3-C4FB-F848-A16E-EF50D38EF95F}">
     <filterColumn colId="0" hiddenButton="1"/>
@@ -5627,6 +5517,46 @@
     <tableColumn id="12" xr3:uid="{EB21D867-EC2A-1046-9372-97B5F5F39552}" name="option_item_name" dataDxfId="19"/>
     <tableColumn id="13" xr3:uid="{83CFFF5F-DD2A-6849-B86D-92DB38FF7001}" name="extra_price" dataDxfId="18"/>
     <tableColumn id="14" xr3:uid="{1CFC430A-35A6-3847-A639-DA9CF813A9A8}" name="option_allergens" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}" name="Table5" displayName="Table5" ref="A1:O50" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="A1:O50" xr:uid="{58DA2B54-9196-8849-95E8-F2DFADBD8518}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+    <filterColumn colId="10" hiddenButton="1"/>
+    <filterColumn colId="11" hiddenButton="1"/>
+    <filterColumn colId="12" hiddenButton="1"/>
+    <filterColumn colId="13" hiddenButton="1"/>
+    <filterColumn colId="14" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="15">
+    <tableColumn id="1" xr3:uid="{1853C437-6A62-6B47-8C9B-564DEA57939A}" name="category" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{7CC90834-B0D1-C849-9B51-B5D9EA77DAA0}" name="sub_category" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{5FF08993-59DB-6349-A6EA-32533F571FF5}" name="name" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{7CF1E11B-4F70-B44E-872E-BCCD8BFE7D9D}" name="price" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{3BF4A478-AEA5-7A41-B357-48C9836E1C80}" name="ingredients" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{E2E7B27E-AAA8-514A-8148-667D740D3AA7}" name="allergens" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{B1097D52-302C-544C-A429-413DED807F5F}" name="description" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{1F2AE8F3-03BD-7B45-A4C7-02179D959056}" name="image_filename" dataDxfId="7"/>
+    <tableColumn id="15" xr3:uid="{49269410-C082-8540-AD51-99931EBA2F5B}" name="option_group_id" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{B8E445A1-F5E1-5047-A344-69C841DD833C}" name="option_group_description" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{21396A92-76A0-2442-B8F3-1DA062E205CC}" name="option_min_quantity" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{557EC8C7-A1C9-F84C-B74C-2B1F02DFEF2A}" name="option_max_quantity" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{E71702D2-99DB-F44C-9D2F-810A07ED5309}" name="option_item_name" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{955FD788-14F2-AA4C-B201-A840E08AD65B}" name="extra_price" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{23C3A0BD-31DD-7249-B139-0E6149C8E21D}" name="option_allergens" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="YEA" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5948,1620 +5878,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67AA6E6-57DF-0445-A312-EF76BC1FF882}">
-  <dimension ref="A1:C16"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="11.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>433</v>
-      </c>
-      <c r="B1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C1" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>241</v>
-      </c>
-      <c r="B2" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B3" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C4" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>437</v>
-      </c>
-      <c r="B5" t="s">
-        <v>438</v>
-      </c>
-      <c r="C5" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>440</v>
-      </c>
-      <c r="C6" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>411</v>
-      </c>
-      <c r="B8" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>413</v>
-      </c>
-      <c r="B9" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>402</v>
-      </c>
-      <c r="C11" t="s">
-        <v>451</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>353</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FC3867-0998-7042-A866-D535493EA32D}">
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="D2" s="1">
-        <v>10.99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="C4" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D4" s="1">
-        <v>14.99</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C5" t="s">
-        <v>242</v>
-      </c>
-      <c r="D5">
-        <v>13.99</v>
-      </c>
-      <c r="E5" t="s">
-        <v>243</v>
-      </c>
-      <c r="F5" t="s">
-        <v>422</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
-        <v>244</v>
-      </c>
-      <c r="D6">
-        <v>12.99</v>
-      </c>
-      <c r="E6" t="s">
-        <v>245</v>
-      </c>
-      <c r="F6" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>246</v>
-      </c>
-      <c r="D7">
-        <v>17.989999999999998</v>
-      </c>
-      <c r="E7" t="s">
-        <v>247</v>
-      </c>
-      <c r="F7" t="s">
-        <v>426</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>248</v>
-      </c>
-      <c r="D8">
-        <v>14.99</v>
-      </c>
-      <c r="E8" t="s">
-        <v>249</v>
-      </c>
-      <c r="F8" t="s">
-        <v>425</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>250</v>
-      </c>
-      <c r="D9">
-        <v>10.99</v>
-      </c>
-      <c r="E9" t="s">
-        <v>251</v>
-      </c>
-      <c r="F9" t="s">
-        <v>424</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6340C06B-693A-1B48-9921-F23546F2EC49}">
-  <dimension ref="A1:O5"/>
-  <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
-        <v>277</v>
-      </c>
-      <c r="B2" s="12"/>
-      <c r="C2" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D2" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D3" s="1">
-        <v>12.99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>270</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>304</v>
-      </c>
-      <c r="D4" s="18">
-        <v>2.99</v>
-      </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-    </row>
-    <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="D5" s="18">
-        <v>2.99</v>
-      </c>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F85CC15-573B-5848-A683-9CAAED797647}">
-  <dimension ref="A1:O9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1"/>
-    <col min="5" max="5" width="44.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="19" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5" style="1" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D2" s="1">
-        <v>9.99</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>314</v>
-      </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="1" t="s">
-        <v>316</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8.99</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2" t="s">
-        <v>318</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>319</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>320</v>
-      </c>
-      <c r="O4" s="2"/>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>313</v>
-      </c>
-      <c r="D5" s="1">
-        <v>8.99</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="D6" s="1">
-        <v>10.99</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>428</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>239</v>
-      </c>
-      <c r="D7" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C8" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="D8" s="1">
-        <v>6.99</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>322</v>
-      </c>
-      <c r="D9" s="1">
-        <v>5.99</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>375</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA28EF5A-AAA6-E243-A364-89A6CC876E03}">
-  <dimension ref="A1:O3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="12" customWidth="1"/>
-    <col min="7" max="8" width="13.83203125" customWidth="1"/>
-    <col min="9" max="9" width="19" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" customWidth="1"/>
-    <col min="11" max="11" width="23.1640625" customWidth="1"/>
-    <col min="12" max="12" width="23.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.5" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="15" width="19.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="10" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="10" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="10" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="10" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="12"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>175</v>
-      </c>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-    </row>
-    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B315ED-1831-0A4D-AF4E-5349EB3E43E8}">
-  <dimension ref="A1:O50"/>
-  <sheetViews>
-    <sheetView topLeftCell="G6" zoomScale="103" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.5" style="6"/>
-    <col min="2" max="2" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="14.5" style="6"/>
-    <col min="7" max="7" width="63.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" style="6"/>
-    <col min="9" max="9" width="27.6640625" style="6" customWidth="1"/>
-    <col min="10" max="10" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.5" style="6" customWidth="1"/>
-    <col min="13" max="13" width="14.5" style="6"/>
-    <col min="14" max="14" width="19.1640625" style="6" customWidth="1"/>
-    <col min="15" max="16384" width="14.5" style="6"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M3" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M4" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>101</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L5" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="M6" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="M7" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="M8" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="K9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="O9" s="6" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="M10" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="J11" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>171</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B14" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="J14" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L14" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="N14" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M15" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M16" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="N16" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M17" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I18" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I19" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="J19" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M20" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="N20" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O20" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M21" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="N21" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O21" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M22" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="N22" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="O22" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I23" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M23" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="N23" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I24" s="6" t="s">
-        <v>144</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="M24" s="6" t="s">
-        <v>146</v>
-      </c>
-      <c r="N24" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M25" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M26" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M27" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M28" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="I29" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>153</v>
-      </c>
-      <c r="N29" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M30" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="N30" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="M31" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
-      <c r="C32" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="E32" s="6" t="s">
-        <v>158</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C34" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C35" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C36" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C37" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C38" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C39" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C40" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C41" s="6" t="s">
-        <v>219</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C42" s="6" t="s">
-        <v>220</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="C43" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>223</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="J43" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="K43" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L43" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="M43" s="6" t="s">
-        <v>228</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M44" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M45" s="6" t="s">
-        <v>230</v>
-      </c>
-      <c r="N45" s="6" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I46" s="6" t="s">
-        <v>232</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="K46" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="M46" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="N46" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M47" s="6" t="s">
-        <v>234</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="M48" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="N48" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M49" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="N49" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
-      <c r="M50" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="N50" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="7" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4635569-6B50-5940-8C00-E7257ADB0B0E}">
   <dimension ref="A1:XFD14"/>
   <sheetViews>
@@ -12216,12 +10532,1271 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6340C06B-693A-1B48-9921-F23546F2EC49}">
+  <dimension ref="A1:O5"/>
+  <sheetViews>
+    <sheetView zoomScale="117" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D2" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="D3" s="1">
+        <v>12.99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>304</v>
+      </c>
+      <c r="D4" s="18">
+        <v>2.99</v>
+      </c>
+      <c r="E4" s="18"/>
+      <c r="F4" s="18"/>
+    </row>
+    <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="C5" s="18" t="s">
+        <v>312</v>
+      </c>
+      <c r="D5" s="18">
+        <v>2.99</v>
+      </c>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F85CC15-573B-5848-A683-9CAAED797647}">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1"/>
+    <col min="5" max="5" width="44.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="19" style="1" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5" style="1" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" style="1" customWidth="1"/>
+    <col min="16" max="16384" width="10.83203125" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" s="1">
+        <v>9.99</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="D3" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="O4" s="2"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="D5" s="1">
+        <v>8.99</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="D6" s="1">
+        <v>10.99</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="D7" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="D8" s="1">
+        <v>6.99</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="D9" s="1">
+        <v>5.99</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA28EF5A-AAA6-E243-A364-89A6CC876E03}">
+  <dimension ref="A1:O3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="12" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="10" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4B315ED-1831-0A4D-AF4E-5349EB3E43E8}">
+  <dimension ref="A1:O50"/>
+  <sheetViews>
+    <sheetView topLeftCell="G6" zoomScale="103" workbookViewId="0">
+      <selection activeCell="J24" sqref="J24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5" style="6"/>
+    <col min="2" max="2" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.1640625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.5" style="6"/>
+    <col min="7" max="7" width="63.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" style="6"/>
+    <col min="9" max="9" width="27.6640625" style="6" customWidth="1"/>
+    <col min="10" max="10" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.5" style="6" customWidth="1"/>
+    <col min="13" max="13" width="14.5" style="6"/>
+    <col min="14" max="14" width="19.1640625" style="6" customWidth="1"/>
+    <col min="15" max="16384" width="14.5" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K4" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L4" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="M6" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7"/>
+      <c r="M7" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7"/>
+      <c r="M8" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="7"/>
+      <c r="M10" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L11" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="N11" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H12" s="7"/>
+      <c r="I12" s="7" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B14" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L14" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N14" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M15" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N16" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="17" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="18" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I18" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="19" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I19" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="20" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M20" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="N20" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O20" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M21" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="N21" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O21" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M22" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="N22" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I23" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="K23" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M23" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I24" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M24" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="N24" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="25" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M25" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="N25" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M26" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="N26" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M27" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="N27" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="28" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M28" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="N28" s="6" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="29" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I29" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="N29" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="N30" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="31" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="M31" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="32" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C32" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="I32" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C36" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C37" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C38" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C39" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C40" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C41" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C42" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C43" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="I43" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="L43" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="M43" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="N43" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M44" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="N45" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="I46" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="M46" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M47" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M48" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="49" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M49" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="N49" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="50" spans="13:14" x14ac:dyDescent="0.25">
+      <c r="M50" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="N50" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E55EDE47-5436-0749-AB83-3D55441C0ECC}">
   <dimension ref="A1:O6"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12293,7 +11868,7 @@
         <v>388</v>
       </c>
       <c r="F2" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
@@ -12310,7 +11885,7 @@
         <v>391</v>
       </c>
       <c r="F3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="J3" t="s">
         <v>390</v>
@@ -12342,7 +11917,7 @@
         <v>393</v>
       </c>
       <c r="F4" t="s">
-        <v>399</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -12376,7 +11951,7 @@
         <v>397</v>
       </c>
       <c r="F6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -12385,7 +11960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C84630-6BE4-A64D-87E5-C7ECC341418B}">
   <dimension ref="A1:O5"/>
   <sheetViews>
@@ -12487,7 +12062,7 @@
         <v>374</v>
       </c>
       <c r="F3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -12504,7 +12079,7 @@
         <v>370</v>
       </c>
       <c r="F4" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -12524,7 +12099,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3BA9BBD-C9D6-C645-B88A-4290D24E034A}">
   <dimension ref="A1:O8"/>
   <sheetViews>
@@ -12616,7 +12191,7 @@
         <v>292</v>
       </c>
       <c r="F3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
@@ -12630,7 +12205,7 @@
         <v>297</v>
       </c>
       <c r="F4" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
@@ -12644,7 +12219,7 @@
         <v>299</v>
       </c>
       <c r="F5" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
@@ -12689,7 +12264,7 @@
         <v>307</v>
       </c>
       <c r="F8" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="G8" t="s">
         <v>311</v>
@@ -12701,7 +12276,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FED334EF-9868-4A4E-84D0-B4BC990B1FD4}">
   <dimension ref="A1:O6"/>
   <sheetViews>
@@ -12815,7 +12390,7 @@
         <v>197</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -12841,7 +12416,7 @@
         <v>252</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="19" x14ac:dyDescent="0.25">
@@ -12858,7 +12433,7 @@
         <v>254</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="19" x14ac:dyDescent="0.25">
@@ -12872,7 +12447,7 @@
         <v>256</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
   </sheetData>
@@ -12884,7 +12459,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{211D9A52-2D82-F545-B3C8-1BEA579932AE}">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -12999,7 +12574,7 @@
         <v>191</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -13022,7 +12597,7 @@
         <v>193</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
@@ -13098,7 +12673,7 @@
         <v>344</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
@@ -13214,7 +12789,7 @@
         <v>325</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="18" spans="3:15" x14ac:dyDescent="0.25">
@@ -13262,7 +12837,7 @@
         <v>0</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="20" spans="3:15" x14ac:dyDescent="0.25">
@@ -13301,13 +12876,13 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="M22" s="19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="N22" s="19">
         <v>0</v>
       </c>
       <c r="O22" s="19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" spans="3:15" x14ac:dyDescent="0.25">
@@ -13334,7 +12909,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67AC912-884F-F44F-A6CD-51118C2A7D9A}">
   <dimension ref="A1:O5"/>
   <sheetViews>
@@ -13421,7 +12996,7 @@
         <v>181</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
@@ -13444,7 +13019,7 @@
         <v>259</v>
       </c>
       <c r="F3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
@@ -13498,7 +13073,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BB6800E-0FE0-C849-BEB9-3BC5DE080FB9}">
   <dimension ref="A1:O4"/>
   <sheetViews>
@@ -13585,7 +13160,7 @@
         <v>183</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -13610,7 +13185,7 @@
         <v>185</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
@@ -13646,4 +13221,222 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71FC3867-0998-7042-A866-D535493EA32D}">
+  <dimension ref="A1:O9"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="16.1640625" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="51.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="19" customWidth="1"/>
+    <col min="10" max="10" width="27.6640625" customWidth="1"/>
+    <col min="11" max="11" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.6640625" customWidth="1"/>
+    <col min="13" max="13" width="21.5" customWidth="1"/>
+    <col min="14" max="14" width="14.33203125" customWidth="1"/>
+    <col min="15" max="15" width="19.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="N1" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="O1" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="D2" s="1">
+        <v>10.99</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14.99</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4" spans="1:15" ht="19" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="D4" s="1">
+        <v>14.99</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D5">
+        <v>13.99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>243</v>
+      </c>
+      <c r="F5" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>244</v>
+      </c>
+      <c r="D6">
+        <v>12.99</v>
+      </c>
+      <c r="E6" t="s">
+        <v>245</v>
+      </c>
+      <c r="F6" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>246</v>
+      </c>
+      <c r="D7">
+        <v>17.989999999999998</v>
+      </c>
+      <c r="E7" t="s">
+        <v>247</v>
+      </c>
+      <c r="F7" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>248</v>
+      </c>
+      <c r="D8">
+        <v>14.99</v>
+      </c>
+      <c r="E8" t="s">
+        <v>249</v>
+      </c>
+      <c r="F8" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>250</v>
+      </c>
+      <c r="D9">
+        <v>10.99</v>
+      </c>
+      <c r="E9" t="s">
+        <v>251</v>
+      </c>
+      <c r="F9" t="s">
+        <v>423</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>